<commit_message>
Agregacion de el sprint burndown 1 y 2, parte grafica
</commit_message>
<xml_diff>
--- a/documentos/PETAPP_SBL_01.xlsx
+++ b/documentos/PETAPP_SBL_01.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="18915" windowHeight="5460"/>
@@ -11,12 +11,15 @@
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId4"/>
+  </externalReferences>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Task</t>
   </si>
@@ -73,6 +76,12 @@
   </si>
   <si>
     <t>Hans Soto Rojas</t>
+  </si>
+  <si>
+    <t>Nro de Horas</t>
+  </si>
+  <si>
+    <t>Carlos Zarate Carpio</t>
   </si>
 </sst>
 </file>
@@ -247,6 +256,286 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-PE"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Sprint </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="es-PE" sz="1800" b="1" i="0" u="none" strike="noStrike" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t>Burndown</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="1800" b="1" i="0" baseline="0">
+                <a:effectLst/>
+              </a:rPr>
+              <a:t> 1</a:t>
+            </a:r>
+            <a:endParaRPr lang="es-PE">
+              <a:effectLst/>
+            </a:endParaRPr>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'SPRINT BACKLOG 1'!$B$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Nro de Horas</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:cat>
+            <c:strRef>
+              <c:f>'SPRINT BACKLOG 1'!$C$4:$I$4</c:f>
+              <c:strCache>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>Day 1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Day 2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Day 3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Day 4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Day 5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Day 6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>Day 7</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'SPRINT BACKLOG 1'!$C$11:$I$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="43389440"/>
+        <c:axId val="43167104"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="43389440"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-PE"/>
+                  <a:t>Nro</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="es-PE" baseline="0"/>
+                  <a:t> Dias</a:t>
+                </a:r>
+                <a:endParaRPr lang="es-PE"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="43167104"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="43167104"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="es-PE"/>
+                  <a:t>Nro de Horas</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="43389440"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1762125</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>128587</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="4 Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="Hoja1"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0" refreshError="1"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -536,10 +825,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:I24"/>
+  <dimension ref="A2:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -732,14 +1021,37 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="10"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
+      <c r="B11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="8">
+        <f>SUM(C6:C10)</f>
+        <v>40</v>
+      </c>
+      <c r="D11" s="8">
+        <f t="shared" ref="D11:I11" si="0">SUM(D6:D10)</f>
+        <v>29</v>
+      </c>
+      <c r="E11" s="8">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="F11" s="8">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="G11" s="8">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="H11" s="8">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="I11" s="8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="11"/>
@@ -770,12 +1082,18 @@
         <v>18</v>
       </c>
     </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>20</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A6:A12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>